<commit_message>
added a CD of USD
</commit_message>
<xml_diff>
--- a/investmentLookup.xlsx
+++ b/investmentLookup.xlsx
@@ -1,31 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAA93A6D-24EC-4B1B-82D9-57793A50B1AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09391E02-F993-46DD-876B-67E135EBB7C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="128">
   <si>
     <t>security_id</t>
   </si>
@@ -405,12 +396,18 @@
   </si>
   <si>
     <t>2963 HK</t>
+  </si>
+  <si>
+    <t>0G5622N</t>
+  </si>
+  <si>
+    <t>AGRICULTURAL BANK OF CHINA LTD/HONG KONG CERTIFICATE OF DEPOSIT ZERO CPN DTD 10/DEC/2020 DUE 10/MAR/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -1002,25 +999,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="28.8">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1043,7 +1040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:7" ht="43.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1061,7 +1058,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30">
+    <row r="3" spans="1:7" ht="28.8">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1081,7 +1078,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="28.8">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1113,7 +1110,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
+    <row r="6" spans="1:7" ht="28.8">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1131,7 +1128,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45">
+    <row r="7" spans="1:7" ht="43.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1148,7 +1145,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45">
+    <row r="8" spans="1:7" ht="43.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1165,7 +1162,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="28.8">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1179,7 +1176,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30">
+    <row r="10" spans="1:7" ht="28.8">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1210,7 +1207,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="28.8">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1318,20 +1315,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:J10"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="101.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1878,8 +1875,18 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="2"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>